<commit_message>
5. Clarify the defenition of the system & 4. modification
</commit_message>
<xml_diff>
--- a/4. Scale management/4.1.3. Функции продукта.xlsx
+++ b/4. Scale management/4.1.3. Функции продукта.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="122">
   <si>
     <t>Подсистема</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Формирование и выдача различных сводок и отчетов</t>
   </si>
   <si>
-    <t>Обеспечение удобной работы с информацией о транспортных средствах</t>
-  </si>
-  <si>
     <t>Хранение информации о сотрудниках</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Необходимость поддерживать в должном состоянии парковки</t>
   </si>
   <si>
-    <t>Система отслеживания доступных парковочных мест</t>
-  </si>
-  <si>
     <t>Оценка оставшегося количества мест на парковке</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>Получение доступа пользователя к парковочному месту</t>
   </si>
   <si>
-    <t xml:space="preserve">Передача данных для формирование отчетов </t>
-  </si>
-  <si>
     <t>Передача данных о новой машине на парковке на сервер</t>
   </si>
   <si>
@@ -354,12 +345,6 @@
     <t>Снижение затрат предприятий на поддержание паркингов</t>
   </si>
   <si>
-    <t>Формирование баз данных клиентов и транспортных средств</t>
-  </si>
-  <si>
-    <t>Хранение общих сведений о транспортных средствах, находящихся на определенной парковке</t>
-  </si>
-  <si>
     <t>Формирование и ведение базы данных о  клиентах</t>
   </si>
   <si>
@@ -381,9 +366,6 @@
     <t xml:space="preserve"> ver 1.1</t>
   </si>
   <si>
-    <t>Формирование и ведение базы данных о транспортных средствах в паркинге</t>
-  </si>
-  <si>
     <t>Оформление брони через телефонное приложение</t>
   </si>
   <si>
@@ -394,6 +376,12 @@
   </si>
   <si>
     <t>Формирование маршрутов до выбранной стоянки</t>
+  </si>
+  <si>
+    <t>Система выбора доступных парковочных мест</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Передача данных для формирования отчетов </t>
   </si>
 </sst>
 </file>
@@ -794,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -848,7 +836,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>11</v>
@@ -863,7 +851,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>14</v>
@@ -875,7 +863,7 @@
     <row r="3" spans="1:9" ht="93.75">
       <c r="A3" s="8"/>
       <c r="B3" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>18</v>
@@ -890,19 +878,19 @@
         <v>44</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75">
       <c r="A4" s="8"/>
       <c r="B4" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
@@ -917,19 +905,19 @@
         <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75">
       <c r="A5" s="8"/>
       <c r="B5" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>18</v>
@@ -944,19 +932,19 @@
         <v>12</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="56.25">
       <c r="A6" s="8"/>
       <c r="B6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>18</v>
@@ -971,13 +959,13 @@
         <v>12</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="70.5" customHeight="1">
@@ -998,7 +986,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1010,7 +998,7 @@
     <row r="8" spans="1:9" ht="75">
       <c r="A8" s="8"/>
       <c r="B8" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>45</v>
@@ -1025,19 +1013,19 @@
         <v>12</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75">
       <c r="A9" s="8"/>
       <c r="B9" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>45</v>
@@ -1052,21 +1040,21 @@
         <v>12</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="78">
+    <row r="10" spans="1:9" ht="58.5">
       <c r="A10" s="8" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>18</v>
@@ -1081,19 +1069,19 @@
         <v>44</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75">
       <c r="A11" s="8"/>
       <c r="B11" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
@@ -1108,19 +1096,19 @@
         <v>13</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75">
       <c r="A12" s="8"/>
       <c r="B12" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>18</v>
@@ -1135,19 +1123,19 @@
         <v>13</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="112.5">
       <c r="A13" s="8"/>
       <c r="B13" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>18</v>
@@ -1162,19 +1150,19 @@
         <v>12</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="75">
       <c r="A14" s="8"/>
       <c r="B14" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>18</v>
@@ -1189,10 +1177,10 @@
         <v>12</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>26</v>
@@ -1200,10 +1188,10 @@
     </row>
     <row r="15" spans="1:9" ht="69.75" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>18</v>
@@ -1218,19 +1206,19 @@
         <v>12</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="75">
       <c r="A16" s="8"/>
       <c r="B16" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>18</v>
@@ -1245,19 +1233,19 @@
         <v>13</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="93.75">
       <c r="A17" s="8"/>
       <c r="B17" s="5" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>18</v>
@@ -1272,13 +1260,13 @@
         <v>44</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="112.5">
@@ -1301,10 +1289,10 @@
         <v>44</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>31</v>
@@ -1328,7 +1316,7 @@
         <v>13</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>29</v>
@@ -1357,7 +1345,7 @@
         <v>44</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>34</v>
@@ -1384,7 +1372,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>37</v>
@@ -1395,10 +1383,10 @@
     </row>
     <row r="22" spans="1:9" ht="78">
       <c r="A22" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
@@ -1413,19 +1401,19 @@
         <v>44</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="75">
       <c r="A23" s="8"/>
       <c r="B23" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -1440,7 +1428,7 @@
         <v>44</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>47</v>
@@ -1452,7 +1440,7 @@
     <row r="24" spans="1:9" ht="75">
       <c r="A24" s="8"/>
       <c r="B24" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>18</v>
@@ -1467,13 +1455,13 @@
         <v>44</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="131.25">
@@ -1494,21 +1482,19 @@
         <v>44</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="112.5">
-      <c r="A26" s="8" t="s">
-        <v>112</v>
-      </c>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="75">
+      <c r="A26" s="8"/>
       <c r="B26" s="5" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>18</v>
@@ -1517,92 +1503,92 @@
         <v>10</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>44</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="75">
-      <c r="A27" s="8"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="93.75">
+      <c r="A27" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="B27" s="5" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="75">
+      <c r="A28" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="93.75">
-      <c r="A28" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="G28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="93.75">
+      <c r="A29" s="8"/>
+      <c r="B29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="75">
-      <c r="A29" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="E29" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>44</v>
@@ -1611,16 +1597,16 @@
         <v>63</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="93.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="56.25">
       <c r="A30" s="8"/>
       <c r="B30" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>18</v>
@@ -1629,73 +1615,46 @@
         <v>15</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>44</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="56.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="75">
       <c r="A31" s="8"/>
       <c r="B31" s="5" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>44</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="75">
-      <c r="A32" s="8"/>
-      <c r="B32" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4 & 5 Modification 2
</commit_message>
<xml_diff>
--- a/4. Scale management/4.1.3. Функции продукта.xlsx
+++ b/4. Scale management/4.1.3. Функции продукта.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="120">
   <si>
     <t>Подсистема</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Решение незначительных проблем и предоставление клиентам интересующей их информации о принципе работа компании</t>
   </si>
   <si>
-    <t>Прочее</t>
-  </si>
-  <si>
     <t>Формирование персональных скидок</t>
   </si>
   <si>
@@ -189,12 +186,6 @@
     <t>Удобство поиска и обработки данных о сотрудниках компании</t>
   </si>
   <si>
-    <t>Повышение взаимодействия сотрудников</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Улучшение отношений в коллективе </t>
-  </si>
-  <si>
     <t>Сохранение конфиденциальости информации</t>
   </si>
   <si>
@@ -225,12 +216,6 @@
     <t>Дополнительные акции и скидки для постоянных пользователей</t>
   </si>
   <si>
-    <t>Использование данных для верификации доступа к парковочному месту</t>
-  </si>
-  <si>
-    <t>Необходимый компонент для адекватной работы системы</t>
-  </si>
-  <si>
     <t>Уверенность клиента в приватности личной информации</t>
   </si>
   <si>
@@ -276,27 +261,12 @@
     <t>ПО для пунктов контроля</t>
   </si>
   <si>
-    <t>Проверка подлинности брони по QR-коду</t>
-  </si>
-  <si>
-    <t>Преддоставление возможности автомату считывать QR-код для верификации</t>
-  </si>
-  <si>
-    <t>Получение доступа пользователя к парковочному месту</t>
-  </si>
-  <si>
     <t>Передача данных о новой машине на парковке на сервер</t>
   </si>
   <si>
     <t>Обеспечение конфиденциальности и сохранности информации, ведения бухгалтерского учета</t>
   </si>
   <si>
-    <t>Обеспечение въезда и выезда пользователя</t>
-  </si>
-  <si>
-    <t>Предоставление возможности въезда и выезда на територию парковки пользователю</t>
-  </si>
-  <si>
     <t>Технические требования к аппаратной части продукта</t>
   </si>
   <si>
@@ -372,9 +342,6 @@
     <t xml:space="preserve">Предоставление возможности оформление брони через приложение на телефоне </t>
   </si>
   <si>
-    <t>Запись информации о машинах</t>
-  </si>
-  <si>
     <t>Формирование маршрутов до выбранной стоянки</t>
   </si>
   <si>
@@ -382,6 +349,33 @@
   </si>
   <si>
     <t xml:space="preserve">Передача данных для формирования отчетов </t>
+  </si>
+  <si>
+    <t>Обеспечение въезда и выезда пользователя с помощью блокираторов и датчиков движения</t>
+  </si>
+  <si>
+    <t>Предоставление возможности въезда и выезда на место парковки пользователю</t>
+  </si>
+  <si>
+    <t>Разработка и внедрения ПО для паркоматов и самих паркоматов</t>
+  </si>
+  <si>
+    <t>Преддоставление возможности клиенту забронировать место находясь уже на парковке. Оплата наличными</t>
+  </si>
+  <si>
+    <t>Возможность использования услуг пользователями без доступа к интернету</t>
+  </si>
+  <si>
+    <t>Управление предприятием</t>
+  </si>
+  <si>
+    <t>Работа с клиентами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Постоянное уведомление клиентов о новых улучшениях продукта </t>
+  </si>
+  <si>
+    <t>Необходимо для поддержания осведомленности пользователей</t>
   </si>
 </sst>
 </file>
@@ -782,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -836,7 +830,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>11</v>
@@ -851,19 +845,19 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="93.75">
       <c r="A3" s="8"/>
       <c r="B3" s="5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>18</v>
@@ -875,22 +869,22 @@
         <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75">
       <c r="A4" s="8"/>
       <c r="B4" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
@@ -905,19 +899,19 @@
         <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="56.25">
       <c r="A5" s="8"/>
       <c r="B5" s="5" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>18</v>
@@ -931,20 +925,20 @@
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>64</v>
+      <c r="G5" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="56.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="70.5" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>18</v>
@@ -953,108 +947,108 @@
         <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>63</v>
+      <c r="G6" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="70.5" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="75">
       <c r="A7" s="8"/>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="75">
       <c r="A8" s="8"/>
       <c r="B8" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>62</v>
+      <c r="G8" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="75">
-      <c r="A9" s="8"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="58.5">
+      <c r="A9" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="B9" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="58.5">
-      <c r="A10" s="8" t="s">
-        <v>120</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="75">
+      <c r="A10" s="8"/>
       <c r="B10" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>18</v>
@@ -1063,79 +1057,79 @@
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="75">
       <c r="A11" s="8"/>
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="112.5">
       <c r="A12" s="8"/>
       <c r="B12" s="5" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="G12" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="112.5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="75">
       <c r="A13" s="8"/>
       <c r="B13" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>18</v>
@@ -1144,54 +1138,54 @@
         <v>12</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="75">
-      <c r="A14" s="8"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="69.75" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="69.75" customHeight="1">
-      <c r="A15" s="8" t="s">
-        <v>85</v>
-      </c>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="93.75">
+      <c r="A15" s="8"/>
       <c r="B15" s="5" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>18</v>
@@ -1200,25 +1194,25 @@
         <v>10</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="93.75">
       <c r="A16" s="8"/>
       <c r="B16" s="5" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>18</v>
@@ -1227,54 +1221,54 @@
         <v>10</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="93.75">
-      <c r="A17" s="8"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="112.5">
+      <c r="A17" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="B17" s="5" t="s">
-        <v>121</v>
+        <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>63</v>
+        <v>43</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="112.5">
-      <c r="A18" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="93.75">
+      <c r="A18" s="8"/>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>18</v>
@@ -1283,25 +1277,27 @@
         <v>15</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>115</v>
+        <v>13</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="93.75">
-      <c r="A19" s="8"/>
+    <row r="19" spans="1:9" ht="75">
+      <c r="A19" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="B19" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>18</v>
@@ -1310,110 +1306,108 @@
         <v>15</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="75">
-      <c r="A20" s="8" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="112.5">
+      <c r="A20" s="8"/>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>63</v>
+        <v>12</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="112.5">
-      <c r="A21" s="8"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="78">
+      <c r="A21" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="78">
-      <c r="A22" s="8" t="s">
-        <v>99</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="75">
+      <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>63</v>
+        <v>43</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="75">
       <c r="A23" s="8"/>
       <c r="B23" s="5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -1425,49 +1419,49 @@
         <v>17</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="75">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="131.25">
       <c r="A24" s="8"/>
       <c r="B24" s="5" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="131.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="75">
       <c r="A25" s="8"/>
       <c r="B25" s="5" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>18</v>
@@ -1479,107 +1473,109 @@
         <v>17</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="75">
-      <c r="A26" s="8"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="93.75">
+      <c r="A26" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="B26" s="5" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="75">
+      <c r="A27" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="75">
+      <c r="A28" s="8"/>
+      <c r="B28" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="93.75">
-      <c r="A27" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="75">
-      <c r="A28" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="D28" s="6" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="93.75">
-      <c r="A29" s="8"/>
+      <c r="A29" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="B29" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>18</v>
@@ -1591,22 +1587,22 @@
         <v>19</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="56.25">
       <c r="A30" s="8"/>
       <c r="B30" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>18</v>
@@ -1618,43 +1614,16 @@
         <v>17</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="75">
-      <c r="A31" s="8"/>
-      <c r="B31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4 & 5 Modification 4
</commit_message>
<xml_diff>
--- a/4. Scale management/4.1.3. Функции продукта.xlsx
+++ b/4. Scale management/4.1.3. Функции продукта.xlsx
@@ -243,9 +243,6 @@
     <t>Сокращение времени в пути</t>
   </si>
   <si>
-    <t>Уведомление пользователя об освободишемся месте на отслеживаемой им парковке</t>
-  </si>
-  <si>
     <t>Информирование пользователей о новых возможностях</t>
   </si>
   <si>
@@ -376,6 +373,9 @@
   </si>
   <si>
     <t>Необходимо для поддержания осведомленности пользователей</t>
+  </si>
+  <si>
+    <t>Уведомление пользователя об освободившемся  месте на отслеживаемой им парковке</t>
   </si>
 </sst>
 </file>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -857,7 +857,7 @@
     <row r="3" spans="1:9" ht="93.75">
       <c r="A3" s="8"/>
       <c r="B3" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>18</v>
@@ -875,16 +875,16 @@
         <v>60</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75">
       <c r="A4" s="8"/>
       <c r="B4" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
@@ -902,10 +902,10 @@
         <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="56.25">
@@ -1018,7 +1018,7 @@
     </row>
     <row r="9" spans="1:9" ht="58.5">
       <c r="A9" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>68</v>
@@ -1075,7 +1075,7 @@
     <row r="11" spans="1:9" ht="75">
       <c r="A11" s="8"/>
       <c r="B11" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
@@ -1102,7 +1102,7 @@
     <row r="12" spans="1:9" ht="112.5">
       <c r="A12" s="8"/>
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>18</v>
@@ -1120,16 +1120,16 @@
         <v>59</v>
       </c>
       <c r="H12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="75">
       <c r="A13" s="8"/>
       <c r="B13" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>18</v>
@@ -1147,7 +1147,7 @@
         <v>59</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>26</v>
@@ -1155,10 +1155,10 @@
     </row>
     <row r="14" spans="1:9" ht="69.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>18</v>
@@ -1176,16 +1176,16 @@
         <v>60</v>
       </c>
       <c r="H14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="93.75">
       <c r="A15" s="8"/>
       <c r="B15" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>18</v>
@@ -1203,16 +1203,16 @@
         <v>60</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="93.75">
       <c r="A16" s="8"/>
       <c r="B16" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>18</v>
@@ -1230,10 +1230,10 @@
         <v>60</v>
       </c>
       <c r="H16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="112.5">
@@ -1256,10 +1256,10 @@
         <v>43</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>31</v>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="21" spans="1:9" ht="78">
       <c r="A21" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>18</v>
@@ -1371,16 +1371,16 @@
         <v>60</v>
       </c>
       <c r="H21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="75">
       <c r="A22" s="8"/>
       <c r="B22" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
@@ -1407,7 +1407,7 @@
     <row r="23" spans="1:9" ht="75">
       <c r="A23" s="8"/>
       <c r="B23" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -1425,10 +1425,10 @@
         <v>60</v>
       </c>
       <c r="H23" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="131.25">
@@ -1452,16 +1452,16 @@
         <v>60</v>
       </c>
       <c r="H24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="75">
       <c r="A25" s="8"/>
       <c r="B25" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>18</v>
@@ -1479,10 +1479,10 @@
         <v>60</v>
       </c>
       <c r="H25" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="93.75">
@@ -1516,7 +1516,7 @@
     </row>
     <row r="27" spans="1:9" ht="75">
       <c r="A27" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>39</v>
@@ -1537,16 +1537,16 @@
         <v>59</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="75">
       <c r="A28" s="8"/>
       <c r="B28" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>44</v>
@@ -1564,15 +1564,15 @@
         <v>59</v>
       </c>
       <c r="H28" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="93.75">
       <c r="A29" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>40</v>

</xml_diff>